<commit_message>
Staging to feature branch
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16785" windowHeight="2625" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16785" windowHeight="2625"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q6"/>
 </workbook>
 </file>
 
@@ -49,22 +48,22 @@
     <t>ESS</t>
   </si>
   <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
+  </si>
+  <si>
+    <t>ABCDe@1234</t>
+  </si>
+  <si>
+    <t>e_name</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
     <t>Peter Mac Anderson</t>
-  </si>
-  <si>
-    <t>Enabled</t>
-  </si>
-  <si>
-    <t>ABCDEF</t>
-  </si>
-  <si>
-    <t>ABCDe@1234</t>
-  </si>
-  <si>
-    <t>e_name</t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
 </sst>
 </file>
@@ -419,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -451,7 +450,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +460,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -481,19 +480,19 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -508,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -533,19 +532,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>